<commit_message>
modify data structure about gbm and hlm
</commit_message>
<xml_diff>
--- a/data/gbm/oil_field_data_for_gbm.xlsx
+++ b/data/gbm/oil_field_data_for_gbm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\PyProjects\simpleLearning\data\gbm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A2B6EE-AC94-477E-AE5F-EB71C6D1F314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D1725B-F044-4F12-A79A-604967E0AC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="792" windowWidth="18468" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="13068" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>氧含量
 (mg/L)</t>
@@ -76,10 +76,6 @@
       <t xml:space="preserve">
 (mm/a)</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>样本序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -143,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -154,7 +150,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -459,17 +454,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="3"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="5" width="6.44140625" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" customWidth="1"/>
@@ -477,18 +472,14 @@
     <col min="9" max="9" width="6.77734375" customWidth="1"/>
     <col min="10" max="10" width="5.77734375" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -514,19 +505,16 @@
       <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
       </c>
       <c r="B2" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6.3</v>
       </c>
       <c r="D2" s="1">
         <v>4.3</v>
@@ -552,19 +540,16 @@
       <c r="K2" s="1">
         <v>7.9</v>
       </c>
-      <c r="L2" s="1">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0.5</v>
       </c>
       <c r="C3" s="1">
-        <v>6.6</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="1">
         <v>1.5</v>
@@ -590,19 +575,16 @@
       <c r="K3" s="1">
         <v>7.9</v>
       </c>
-      <c r="L3" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>6.8</v>
       </c>
       <c r="D4" s="1">
         <v>3.7</v>
@@ -628,19 +610,16 @@
       <c r="K4" s="1">
         <v>7.9</v>
       </c>
-      <c r="L4" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
       </c>
       <c r="B5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6.5</v>
       </c>
       <c r="D5" s="1">
         <v>4.0999999999999996</v>
@@ -666,19 +645,16 @@
       <c r="K5" s="1">
         <v>7.9</v>
       </c>
-      <c r="L5" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
+    </row>
+    <row r="6" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
       </c>
       <c r="B6" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.6</v>
-      </c>
-      <c r="C6" s="1">
-        <v>6.1</v>
       </c>
       <c r="D6" s="1">
         <v>5.8</v>
@@ -704,19 +680,16 @@
       <c r="K6" s="1">
         <v>7.7</v>
       </c>
-      <c r="L6" s="1">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
+    </row>
+    <row r="7" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
       </c>
       <c r="B7" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.6</v>
       </c>
       <c r="D7" s="1">
         <v>5.0999999999999996</v>
@@ -742,19 +715,16 @@
       <c r="K7" s="1">
         <v>7.8</v>
       </c>
-      <c r="L7" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
+    </row>
+    <row r="8" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
       </c>
       <c r="B8" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7.3</v>
       </c>
       <c r="D8" s="1">
         <v>2.9</v>
@@ -780,19 +750,16 @@
       <c r="K8" s="1">
         <v>7.8</v>
       </c>
-      <c r="L8" s="1">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
+    </row>
+    <row r="9" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
       </c>
       <c r="B9" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6.1</v>
       </c>
       <c r="D9" s="1">
         <v>5.2</v>
@@ -818,19 +785,16 @@
       <c r="K9" s="1">
         <v>7.8</v>
       </c>
-      <c r="L9" s="1">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
+    </row>
+    <row r="10" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
       </c>
       <c r="B10" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="C10" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>6.2</v>
       </c>
       <c r="D10" s="1">
         <v>3.1</v>
@@ -856,19 +820,16 @@
       <c r="K10" s="1">
         <v>7.8</v>
       </c>
-      <c r="L10" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
       </c>
       <c r="B11" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6.8</v>
       </c>
       <c r="D11" s="1">
         <v>3.3</v>
@@ -894,19 +855,16 @@
       <c r="K11" s="1">
         <v>7.7</v>
       </c>
-      <c r="L11" s="1">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
+    </row>
+    <row r="12" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
       </c>
       <c r="B12" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6.5</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
@@ -932,19 +890,16 @@
       <c r="K12" s="1">
         <v>8</v>
       </c>
-      <c r="L12" s="1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
+    </row>
+    <row r="13" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
       </c>
       <c r="B13" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C13" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>6.7</v>
       </c>
       <c r="D13" s="1">
         <v>3.7</v>
@@ -970,19 +925,16 @@
       <c r="K13" s="1">
         <v>7.9</v>
       </c>
-      <c r="L13" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
+    </row>
+    <row r="14" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
       </c>
       <c r="B14" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.6</v>
-      </c>
-      <c r="C14" s="1">
-        <v>6.4</v>
       </c>
       <c r="D14" s="1">
         <v>4.5</v>
@@ -1008,19 +960,16 @@
       <c r="K14" s="1">
         <v>7.8</v>
       </c>
-      <c r="L14" s="1">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
+    </row>
+    <row r="15" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
       </c>
       <c r="B15" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.4</v>
-      </c>
-      <c r="C15" s="1">
-        <v>6.6</v>
       </c>
       <c r="D15" s="1">
         <v>3.8</v>
@@ -1046,19 +995,16 @@
       <c r="K15" s="1">
         <v>7.9</v>
       </c>
-      <c r="L15" s="1">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
+    </row>
+    <row r="16" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>14</v>
       </c>
       <c r="B16" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>6.2</v>
       </c>
       <c r="D16" s="1">
         <v>3.9</v>
@@ -1084,19 +1030,16 @@
       <c r="K16" s="1">
         <v>7.4</v>
       </c>
-      <c r="L16" s="1">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
+    </row>
+    <row r="17" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>15</v>
       </c>
       <c r="B17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.5</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6.4</v>
       </c>
       <c r="D17" s="1">
         <v>4.0999999999999996</v>
@@ -1122,19 +1065,16 @@
       <c r="K17" s="1">
         <v>7.6</v>
       </c>
-      <c r="L17" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
+    </row>
+    <row r="18" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>16</v>
       </c>
       <c r="B18" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="C18" s="1">
         <v>0.8</v>
-      </c>
-      <c r="C18" s="1">
-        <v>6.8</v>
       </c>
       <c r="D18" s="1">
         <v>3.9</v>
@@ -1160,19 +1100,16 @@
       <c r="K18" s="1">
         <v>7.5</v>
       </c>
-      <c r="L18" s="1">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
+    </row>
+    <row r="19" spans="1:11" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>17</v>
       </c>
       <c r="B19" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="C19" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C19" s="1">
-        <v>6.9</v>
       </c>
       <c r="D19" s="1">
         <v>3.6</v>
@@ -1197,9 +1134,6 @@
       </c>
       <c r="K19" s="1">
         <v>7.9</v>
-      </c>
-      <c r="L19" s="1">
-        <v>0.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>